<commit_message>
Improvements after meeting with Ruud
</commit_message>
<xml_diff>
--- a/Data/FodstadData.xlsx
+++ b/Data/FodstadData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E0EF2E-9DAC-4D40-9BFE-2844E21D69EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058B3F4A-4767-8441-8B95-FCECC6ADABB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26860" activeTab="6" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26860" activeTab="4" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualisation" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
   <si>
     <t>ID</t>
   </si>
@@ -400,6 +400,18 @@
   </si>
   <si>
     <t>Niet op Gassco</t>
+  </si>
+  <si>
+    <t>TSO entry costs Gas</t>
+  </si>
+  <si>
+    <t>TSO exit costs Gas</t>
+  </si>
+  <si>
+    <t>TSO entry costs Hydrogen</t>
+  </si>
+  <si>
+    <t>TSO exit costs Hydrogen</t>
   </si>
 </sst>
 </file>
@@ -499,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -559,13 +571,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -586,22 +629,19 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1028,7 +1068,7 @@
     </row>
     <row r="2" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
-        <f>Nodes!H2</f>
+        <f>Nodes!J2</f>
         <v>Production Capacity Gas</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1040,7 +1080,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
-        <f>Nodes!K2</f>
+        <f>Nodes!M2</f>
         <v>Production Costs Gas</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1050,7 +1090,7 @@
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
-        <f>Nodes!L2</f>
+        <f>Nodes!N2</f>
         <v>Storage Capacity Gas</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1060,7 +1100,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
-        <f>Nodes!M2</f>
+        <f>Nodes!O2</f>
         <v>Entry Storage Costs Gas</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1070,7 +1110,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
-        <f>Nodes!N2</f>
+        <f>Nodes!P2</f>
         <v>Entry Costs Gas Stage 1</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1080,7 +1120,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
-        <f>Nodes!O2</f>
+        <f>Nodes!Q2</f>
         <v>Exit Costs Gas Stage 1</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1124,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3F5746-A1B1-6F4F-9762-CACD4A91B5F2}">
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,32 +1178,35 @@
     <col min="4" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.1640625" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1175,34 +1218,38 @@
         <f>Commodities!B2</f>
         <v>gas</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="19" t="str">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="18" t="str">
         <f>Commodities!B3</f>
         <v>hydrogen</v>
       </c>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="21"/>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="20"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1221,83 +1268,95 @@
       <c r="F2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="V2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1315,54 +1374,54 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="13">
-        <f>($H$23-$H$22)/3</f>
+      <c r="H3" s="2">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5</v>
+      </c>
+      <c r="J3" s="13">
+        <f>($J$23-$J$22)/3</f>
         <v>24.933333333333337</v>
       </c>
-      <c r="I3" s="13">
+      <c r="K3" s="13">
         <v>500</v>
       </c>
-      <c r="J3" s="13">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="L3" s="13">
         <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R3" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S3" s="2">
-        <v>5</v>
-      </c>
-      <c r="T3" s="3">
-        <v>0</v>
-      </c>
-      <c r="U3" s="3">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T3" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1.5</v>
       </c>
       <c r="V3" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W3" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X3" s="3">
         <v>0</v>
@@ -1388,8 +1447,20 @@
       <c r="AE3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1409,53 +1480,53 @@
       <c r="G4" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>5</v>
+      </c>
+      <c r="J4" s="13">
         <v>27</v>
       </c>
-      <c r="I4" s="13">
+      <c r="K4" s="13">
         <v>500</v>
       </c>
-      <c r="J4" s="13">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="L4" s="13">
         <v>0</v>
       </c>
       <c r="M4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R4" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S4" s="2">
-        <v>5</v>
-      </c>
-      <c r="T4" s="3">
-        <v>0</v>
-      </c>
-      <c r="U4" s="3">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1.5</v>
       </c>
       <c r="V4" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W4" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X4" s="3">
         <v>0</v>
@@ -1481,8 +1552,20 @@
       <c r="AE4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1502,53 +1585,53 @@
       <c r="G5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
-      <c r="I5" s="13">
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0</v>
+      </c>
+      <c r="K5" s="13">
         <v>500</v>
       </c>
-      <c r="J5" s="13">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="L5" s="13">
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R5" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S5" s="2">
-        <v>5</v>
-      </c>
-      <c r="T5" s="3">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U5" s="2">
+        <v>1.5</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X5" s="3">
         <v>0</v>
@@ -1574,8 +1657,20 @@
       <c r="AE5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1593,54 +1688,54 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="13">
-        <f>($H$23-$H$22)/3</f>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5</v>
+      </c>
+      <c r="J6" s="13">
+        <f>($J$23-$J$22)/3</f>
         <v>24.933333333333337</v>
       </c>
-      <c r="I6" s="13">
+      <c r="K6" s="13">
         <v>500</v>
       </c>
-      <c r="J6" s="13">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="L6" s="13">
         <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R6" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S6" s="2">
-        <v>5</v>
-      </c>
-      <c r="T6" s="3">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U6" s="2">
+        <v>1.5</v>
       </c>
       <c r="V6" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W6" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X6" s="3">
         <v>0</v>
@@ -1666,8 +1761,20 @@
       <c r="AE6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1687,53 +1794,53 @@
       <c r="G7" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>5</v>
+      </c>
+      <c r="J7" s="13">
         <v>143</v>
       </c>
-      <c r="I7" s="13">
+      <c r="K7" s="13">
         <v>500</v>
       </c>
-      <c r="J7" s="13">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="L7" s="13">
         <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R7" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S7" s="2">
-        <v>5</v>
-      </c>
-      <c r="T7" s="3">
-        <v>0</v>
-      </c>
-      <c r="U7" s="3">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1.5</v>
       </c>
       <c r="V7" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W7" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X7" s="3">
         <v>0</v>
@@ -1759,8 +1866,20 @@
       <c r="AE7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1778,53 +1897,53 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="13">
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="13">
         <v>84</v>
       </c>
-      <c r="I8" s="13">
+      <c r="K8" s="13">
         <v>500</v>
       </c>
-      <c r="J8" s="13">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="L8" s="13">
         <v>0</v>
       </c>
       <c r="M8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R8" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S8" s="2">
-        <v>5</v>
-      </c>
-      <c r="T8" s="3">
-        <v>0</v>
-      </c>
-      <c r="U8" s="3">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1.5</v>
       </c>
       <c r="V8" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W8" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X8" s="3">
         <v>0</v>
@@ -1850,8 +1969,20 @@
       <c r="AE8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1869,54 +2000,54 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="13">
-        <f>($H$23-$H$22)/3</f>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>5</v>
+      </c>
+      <c r="J9" s="13">
+        <f>($J$23-$J$22)/3</f>
         <v>24.933333333333337</v>
       </c>
-      <c r="I9" s="13">
+      <c r="K9" s="13">
         <v>500</v>
       </c>
-      <c r="J9" s="13">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="L9" s="13">
         <v>0</v>
       </c>
       <c r="M9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R9" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S9" s="2">
-        <v>5</v>
-      </c>
-      <c r="T9" s="3">
-        <v>0</v>
-      </c>
-      <c r="U9" s="3">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1.5</v>
       </c>
       <c r="V9" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W9" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X9" s="3">
         <v>0</v>
@@ -1942,8 +2073,20 @@
       <c r="AE9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1963,53 +2106,53 @@
       <c r="G10" t="s">
         <v>68</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
+      <c r="J10" s="13">
         <v>21.2</v>
       </c>
-      <c r="I10" s="13">
+      <c r="K10" s="13">
         <v>500</v>
       </c>
-      <c r="J10" s="13">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="L10" s="13">
         <v>0</v>
       </c>
       <c r="M10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R10" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S10" s="2">
-        <v>5</v>
-      </c>
-      <c r="T10" s="3">
-        <v>0</v>
-      </c>
-      <c r="U10" s="3">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U10" s="2">
+        <v>1.5</v>
       </c>
       <c r="V10" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W10" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X10" s="3">
         <v>0</v>
@@ -2035,8 +2178,20 @@
       <c r="AE10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2055,76 +2210,76 @@
       <c r="F11" s="1"/>
       <c r="G11" s="11"/>
       <c r="H11" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I11" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
         <v>500</v>
       </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
       <c r="M11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R11" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S11" s="2">
-        <v>5</v>
-      </c>
-      <c r="T11" s="3">
-        <f t="shared" ref="T11:T20" si="0">H11</f>
-        <v>0</v>
-      </c>
-      <c r="U11" s="3">
-        <f t="shared" ref="U11:U20" si="1">K11</f>
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U11" s="2">
+        <v>1.5</v>
       </c>
       <c r="V11" s="3">
-        <f t="shared" ref="V11:V20" si="2">L11</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W11" s="3">
-        <f t="shared" ref="W11:W20" si="3">M11</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X11" s="3">
-        <f t="shared" ref="X11:X20" si="4">N11</f>
-        <v>1</v>
+        <f t="shared" ref="X11:X20" si="0">J11</f>
+        <v>0</v>
       </c>
       <c r="Y11" s="3">
-        <f t="shared" ref="Y11:Y20" si="5">O11</f>
+        <f t="shared" ref="Y11:Y20" si="1">M11</f>
         <v>1</v>
       </c>
       <c r="Z11" s="3">
+        <f t="shared" ref="Z11:Z20" si="2">N11</f>
         <v>0</v>
       </c>
       <c r="AA11" s="3">
+        <f t="shared" ref="AA11:AA20" si="3">O11</f>
         <v>0</v>
       </c>
       <c r="AB11" s="3">
-        <v>0</v>
+        <f t="shared" ref="AB11:AB20" si="4">P11</f>
+        <v>1</v>
       </c>
       <c r="AC11" s="3">
-        <v>0</v>
+        <f t="shared" ref="AC11:AC20" si="5">Q11</f>
+        <v>1</v>
       </c>
       <c r="AD11" s="3">
         <v>0</v>
@@ -2132,8 +2287,20 @@
       <c r="AE11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2150,87 +2317,99 @@
         <v>15</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
         <v>500</v>
       </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
       <c r="M12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R12" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S12" s="2">
-        <v>5</v>
-      </c>
-      <c r="T12" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T12" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U12" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V12" s="3">
+        <v>5</v>
+      </c>
+      <c r="W12" s="3">
+        <v>5</v>
+      </c>
+      <c r="X12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U12" s="3">
+      <c r="Y12" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V12" s="3">
+      <c r="Z12" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W12" s="3">
+      <c r="AA12" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X12" s="3">
+      <c r="AB12" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y12" s="3">
+      <c r="AC12" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="3">
-        <v>0</v>
-      </c>
       <c r="AD12" s="3">
         <v>0</v>
       </c>
       <c r="AE12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2247,87 +2426,99 @@
         <v>10</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I13" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
         <v>500</v>
       </c>
-      <c r="K13" s="2">
-        <v>1</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0</v>
-      </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R13" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S13" s="2">
-        <v>5</v>
-      </c>
-      <c r="T13" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T13" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U13" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V13" s="3">
+        <v>5</v>
+      </c>
+      <c r="W13" s="3">
+        <v>5</v>
+      </c>
+      <c r="X13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U13" s="3">
+      <c r="Y13" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V13" s="3">
+      <c r="Z13" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W13" s="3">
+      <c r="AA13" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X13" s="3">
+      <c r="AB13" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y13" s="3">
+      <c r="AC13" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="3">
-        <v>0</v>
-      </c>
       <c r="AD13" s="3">
         <v>0</v>
       </c>
       <c r="AE13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2344,87 +2535,99 @@
         <v>5</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I14" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
         <v>500</v>
       </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0</v>
-      </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R14" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S14" s="2">
-        <v>5</v>
-      </c>
-      <c r="T14" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V14" s="3">
+        <v>5</v>
+      </c>
+      <c r="W14" s="3">
+        <v>5</v>
+      </c>
+      <c r="X14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U14" s="3">
+      <c r="Y14" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V14" s="3">
+      <c r="Z14" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W14" s="3">
+      <c r="AA14" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X14" s="3">
+      <c r="AB14" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y14" s="3">
+      <c r="AC14" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="3">
-        <v>0</v>
-      </c>
       <c r="AD14" s="3">
         <v>0</v>
       </c>
       <c r="AE14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2443,87 +2646,99 @@
       <c r="F15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I15" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J15" s="2">
         <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2">
         <v>0</v>
       </c>
       <c r="M15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R15" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S15" s="2">
-        <v>5</v>
-      </c>
-      <c r="T15" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V15" s="3">
+        <v>5</v>
+      </c>
+      <c r="W15" s="3">
+        <v>5</v>
+      </c>
+      <c r="X15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U15" s="3">
+      <c r="Y15" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V15" s="3">
+      <c r="Z15" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W15" s="3">
+      <c r="AA15" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X15" s="3">
+      <c r="AB15" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="AC15" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="3">
-        <v>0</v>
-      </c>
       <c r="AD15" s="3">
         <v>0</v>
       </c>
       <c r="AE15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2542,87 +2757,99 @@
       <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I16" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
       </c>
       <c r="K16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
       </c>
       <c r="M16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R16" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S16" s="2">
-        <v>5</v>
-      </c>
-      <c r="T16" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T16" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U16" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V16" s="3">
+        <v>5</v>
+      </c>
+      <c r="W16" s="3">
+        <v>5</v>
+      </c>
+      <c r="X16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U16" s="3">
+      <c r="Y16" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V16" s="3">
+      <c r="Z16" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W16" s="3">
+      <c r="AA16" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X16" s="3">
+      <c r="AB16" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="AC16" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="3">
-        <v>0</v>
-      </c>
       <c r="AD16" s="3">
         <v>0</v>
       </c>
       <c r="AE16" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2641,87 +2868,99 @@
       <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="11"/>
       <c r="H17" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I17" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J17" s="2">
         <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="2">
         <v>0</v>
       </c>
       <c r="M17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R17" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S17" s="2">
-        <v>5</v>
-      </c>
-      <c r="T17" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T17" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U17" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V17" s="3">
+        <v>5</v>
+      </c>
+      <c r="W17" s="3">
+        <v>5</v>
+      </c>
+      <c r="X17" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U17" s="3">
+      <c r="Y17" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V17" s="3">
+      <c r="Z17" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W17" s="3">
+      <c r="AA17" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X17" s="3">
+      <c r="AB17" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y17" s="3">
+      <c r="AC17" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z17" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="3">
-        <v>0</v>
-      </c>
       <c r="AD17" s="3">
         <v>0</v>
       </c>
       <c r="AE17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2740,87 +2979,99 @@
       <c r="F18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I18" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J18" s="2">
         <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
       </c>
       <c r="M18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R18" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S18" s="2">
-        <v>5</v>
-      </c>
-      <c r="T18" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T18" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U18" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V18" s="3">
+        <v>5</v>
+      </c>
+      <c r="W18" s="3">
+        <v>5</v>
+      </c>
+      <c r="X18" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U18" s="3">
+      <c r="Y18" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V18" s="3">
+      <c r="Z18" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W18" s="3">
+      <c r="AA18" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X18" s="3">
+      <c r="AB18" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y18" s="3">
+      <c r="AC18" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="3">
-        <v>0</v>
-      </c>
       <c r="AD18" s="3">
         <v>0</v>
       </c>
       <c r="AE18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2839,87 +3090,99 @@
       <c r="F19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I19" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J19" s="2">
         <v>0</v>
       </c>
       <c r="K19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="2">
         <v>0</v>
       </c>
       <c r="M19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R19" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S19" s="2">
-        <v>5</v>
-      </c>
-      <c r="T19" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T19" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U19" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V19" s="3">
+        <v>5</v>
+      </c>
+      <c r="W19" s="3">
+        <v>5</v>
+      </c>
+      <c r="X19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U19" s="3">
+      <c r="Y19" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V19" s="3">
+      <c r="Z19" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W19" s="3">
+      <c r="AA19" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X19" s="3">
+      <c r="AB19" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y19" s="3">
+      <c r="AC19" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z19" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="3">
-        <v>0</v>
-      </c>
       <c r="AD19" s="3">
         <v>0</v>
       </c>
       <c r="AE19" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2936,107 +3199,119 @@
         <v>25</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="11"/>
       <c r="H20" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I20" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J20" s="2">
         <v>0</v>
       </c>
       <c r="K20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
       </c>
       <c r="M20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R20" s="2">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="S20" s="2">
-        <v>5</v>
-      </c>
-      <c r="T20" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T20" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U20" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V20" s="3">
+        <v>5</v>
+      </c>
+      <c r="W20" s="3">
+        <v>5</v>
+      </c>
+      <c r="X20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U20" s="3">
+      <c r="Y20" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="V20" s="3">
+      <c r="Z20" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W20" s="3">
+      <c r="AA20" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X20" s="3">
+      <c r="AB20" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y20" s="3">
+      <c r="AC20" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Z20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="3">
-        <v>0</v>
-      </c>
       <c r="AD20" s="3">
         <v>0</v>
       </c>
       <c r="AE20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
         <v>71</v>
       </c>
-      <c r="H22">
-        <f>SUM(H10+H8+H7+H5+H4)</f>
+      <c r="J22">
+        <f>SUM(J10+J8+J7+J5+J4)</f>
         <v>275.2</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="G23" t="s">
         <v>70</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>350</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H1:S1"/>
-    <mergeCell ref="T1:AE1"/>
+    <mergeCell ref="H1:U1"/>
+    <mergeCell ref="V1:AI1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3048,7 +3323,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3062,46 +3337,47 @@
       <c r="A1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="24">
-        <v>1</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="B1" s="23">
+        <f>Parameters!B5+1</f>
+        <v>2</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="24">
-        <v>1</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="B2" s="23">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -3489,8 +3765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7506CF-850A-ED42-956F-025E5A994524}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3504,105 +3780,107 @@
       <c r="A1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="24">
-        <v>2</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24">
+      <c r="B1" s="23">
+        <f>Parameters!B5*(1+Parameters!B6)+1</f>
         <v>3</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23">
+        <f>B1+Parameters!B5+1</f>
+        <v>5</v>
+      </c>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.5</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23">
         <v>0.5</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="25">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="25">
-        <v>1</v>
-      </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="27"/>
+      <c r="B3" s="24">
+        <v>2</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="24">
+        <v>2</v>
+      </c>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="26"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="22" t="str">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="21" t="str">
         <f>B4</f>
         <v>gas or mix</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="23" t="str">
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="22" t="str">
         <f>F4</f>
         <v>pure hydrogen</v>
       </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -4245,7 +4523,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4334,8 +4612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902688A-D2A3-854F-B341-C0BEC53AF991}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E22"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Our data works now
</commit_message>
<xml_diff>
--- a/Data/FodstadData.xlsx
+++ b/Data/FodstadData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38EB058-2698-A943-89DA-BBF6652BB1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D883B4-4E9D-C349-BC28-4096DC8BEC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26860" activeTab="2" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="126">
   <si>
     <t>ID</t>
   </si>
@@ -699,7 +699,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -736,6 +736,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -751,22 +752,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -779,6 +771,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1161,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F599A445-15C0-AB40-A0A7-7DAECA950535}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,90 +1173,81 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1421,7 @@
   <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1476,40 +1468,40 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="28" t="str">
+      <c r="H1" s="29" t="str">
         <f>Commodities!B2</f>
         <v>gas</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="30" t="str">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="31" t="str">
         <f>Commodities!B3</f>
         <v>hydrogen</v>
       </c>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="33"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1668,16 +1660,16 @@
         <v>1</v>
       </c>
       <c r="R3" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S3" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T3" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U3" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V3" s="3">
         <v>5</v>
@@ -1773,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="R4" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S4" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T4" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U4" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V4" s="3">
         <v>5</v>
@@ -1878,16 +1870,16 @@
         <v>1</v>
       </c>
       <c r="R5" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S5" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T5" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U5" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V5" s="3">
         <v>5</v>
@@ -1982,16 +1974,16 @@
         <v>1</v>
       </c>
       <c r="R6" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S6" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T6" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U6" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V6" s="3">
         <v>5</v>
@@ -2087,16 +2079,16 @@
         <v>1</v>
       </c>
       <c r="R7" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S7" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T7" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U7" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V7" s="3">
         <v>5</v>
@@ -2190,16 +2182,16 @@
         <v>1</v>
       </c>
       <c r="R8" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S8" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T8" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U8" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V8" s="3">
         <v>5</v>
@@ -2294,16 +2286,16 @@
         <v>1</v>
       </c>
       <c r="R9" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S9" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T9" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U9" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V9" s="3">
         <v>5</v>
@@ -2399,16 +2391,16 @@
         <v>1</v>
       </c>
       <c r="R10" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S10" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T10" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U10" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V10" s="3">
         <v>5</v>
@@ -2502,16 +2494,16 @@
         <v>1</v>
       </c>
       <c r="R11" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S11" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T11" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U11" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V11" s="3">
         <v>5</v>
@@ -2607,16 +2599,16 @@
         <v>1</v>
       </c>
       <c r="R12" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S12" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T12" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U12" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V12" s="3">
         <v>5</v>
@@ -2712,16 +2704,16 @@
         <v>1</v>
       </c>
       <c r="R13" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S13" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T13" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U13" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V13" s="3">
         <v>5</v>
@@ -2817,16 +2809,16 @@
         <v>1</v>
       </c>
       <c r="R14" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S14" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T14" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U14" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V14" s="3">
         <v>5</v>
@@ -2924,16 +2916,16 @@
         <v>1</v>
       </c>
       <c r="R15" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S15" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T15" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U15" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V15" s="3">
         <v>5</v>
@@ -3032,16 +3024,16 @@
         <v>1</v>
       </c>
       <c r="R16" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S16" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T16" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U16" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V16" s="3">
         <v>5</v>
@@ -3140,16 +3132,16 @@
         <v>1</v>
       </c>
       <c r="R17" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S17" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T17" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U17" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V17" s="3">
         <v>5</v>
@@ -3248,16 +3240,16 @@
         <v>1</v>
       </c>
       <c r="R18" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S18" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T18" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U18" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V18" s="3">
         <v>5</v>
@@ -3356,16 +3348,16 @@
         <v>1</v>
       </c>
       <c r="R19" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S19" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T19" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U19" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V19" s="3">
         <v>5</v>
@@ -3462,16 +3454,16 @@
         <v>1</v>
       </c>
       <c r="R20" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S20" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T20" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="U20" s="2">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="V20" s="3">
         <v>5</v>
@@ -3565,98 +3557,98 @@
       <c r="A1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="36">
         <v>2</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36">
         <f>B1+Parameters!$B$5</f>
         <v>6</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33">
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36">
         <f>J1+Parameters!$B$5</f>
         <v>10</v>
       </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33">
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36">
         <f>R1+Parameters!$B$5</f>
         <v>14</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="36">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36">
         <f>3/24</f>
         <v>0.125</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33">
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36">
         <f>6/24</f>
         <v>0.25</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33">
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36">
         <f>3/24</f>
         <v>0.125</v>
       </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
@@ -5103,6 +5095,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="Z2:AG2"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B1:I1"/>
@@ -5111,14 +5111,6 @@
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="Z2:AG2"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="AD3:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5143,527 +5135,527 @@
       <c r="A1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="36">
         <v>18</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36">
         <f>B1+Parameters!$B$5</f>
         <v>22</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33">
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36">
         <f>J1+Parameters!$B$5</f>
         <v>26</v>
       </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33">
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36">
         <f>R1+Parameters!$B$5</f>
         <v>30</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33">
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36">
         <f>Z1+Parameters!$B$5</f>
         <v>34</v>
       </c>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33">
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36">
         <f>AH1+Parameters!$B$5</f>
         <v>38</v>
       </c>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
-      <c r="AS1" s="33"/>
-      <c r="AT1" s="33"/>
-      <c r="AU1" s="33"/>
-      <c r="AV1" s="33"/>
-      <c r="AW1" s="33"/>
-      <c r="AX1" s="33">
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="36"/>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="36"/>
+      <c r="AV1" s="36"/>
+      <c r="AW1" s="36"/>
+      <c r="AX1" s="36">
         <f>AP1+Parameters!$B$5</f>
         <v>42</v>
       </c>
-      <c r="AY1" s="33"/>
-      <c r="AZ1" s="33"/>
-      <c r="BA1" s="33"/>
-      <c r="BB1" s="33"/>
-      <c r="BC1" s="33"/>
-      <c r="BD1" s="33"/>
-      <c r="BE1" s="33"/>
-      <c r="BF1" s="33">
+      <c r="AY1" s="36"/>
+      <c r="AZ1" s="36"/>
+      <c r="BA1" s="36"/>
+      <c r="BB1" s="36"/>
+      <c r="BC1" s="36"/>
+      <c r="BD1" s="36"/>
+      <c r="BE1" s="36"/>
+      <c r="BF1" s="36">
         <f>AX1+Parameters!$B$5</f>
         <v>46</v>
       </c>
-      <c r="BG1" s="33"/>
-      <c r="BH1" s="33"/>
-      <c r="BI1" s="33"/>
-      <c r="BJ1" s="33"/>
-      <c r="BK1" s="33"/>
-      <c r="BL1" s="33"/>
-      <c r="BM1" s="33"/>
-      <c r="BN1" s="33">
+      <c r="BG1" s="36"/>
+      <c r="BH1" s="36"/>
+      <c r="BI1" s="36"/>
+      <c r="BJ1" s="36"/>
+      <c r="BK1" s="36"/>
+      <c r="BL1" s="36"/>
+      <c r="BM1" s="36"/>
+      <c r="BN1" s="36">
         <f>BF1+Parameters!$B$5</f>
         <v>50</v>
       </c>
-      <c r="BO1" s="33"/>
-      <c r="BP1" s="33"/>
-      <c r="BQ1" s="33"/>
-      <c r="BR1" s="33"/>
-      <c r="BS1" s="33"/>
-      <c r="BT1" s="33"/>
-      <c r="BU1" s="33"/>
-      <c r="BV1" s="33">
+      <c r="BO1" s="36"/>
+      <c r="BP1" s="36"/>
+      <c r="BQ1" s="36"/>
+      <c r="BR1" s="36"/>
+      <c r="BS1" s="36"/>
+      <c r="BT1" s="36"/>
+      <c r="BU1" s="36"/>
+      <c r="BV1" s="36">
         <f>BN1+Parameters!$B$5</f>
         <v>54</v>
       </c>
-      <c r="BW1" s="33"/>
-      <c r="BX1" s="33"/>
-      <c r="BY1" s="33"/>
-      <c r="BZ1" s="33"/>
-      <c r="CA1" s="33"/>
-      <c r="CB1" s="33"/>
-      <c r="CC1" s="33"/>
-      <c r="CD1" s="33">
+      <c r="BW1" s="36"/>
+      <c r="BX1" s="36"/>
+      <c r="BY1" s="36"/>
+      <c r="BZ1" s="36"/>
+      <c r="CA1" s="36"/>
+      <c r="CB1" s="36"/>
+      <c r="CC1" s="36"/>
+      <c r="CD1" s="36">
         <f>BV1+Parameters!$B$5</f>
         <v>58</v>
       </c>
-      <c r="CE1" s="33"/>
-      <c r="CF1" s="33"/>
-      <c r="CG1" s="33"/>
-      <c r="CH1" s="33"/>
-      <c r="CI1" s="33"/>
-      <c r="CJ1" s="33"/>
-      <c r="CK1" s="33"/>
-      <c r="CL1" s="33">
+      <c r="CE1" s="36"/>
+      <c r="CF1" s="36"/>
+      <c r="CG1" s="36"/>
+      <c r="CH1" s="36"/>
+      <c r="CI1" s="36"/>
+      <c r="CJ1" s="36"/>
+      <c r="CK1" s="36"/>
+      <c r="CL1" s="36">
         <f>CD1+Parameters!$B$5</f>
         <v>62</v>
       </c>
-      <c r="CM1" s="33"/>
-      <c r="CN1" s="33"/>
-      <c r="CO1" s="33"/>
-      <c r="CP1" s="33"/>
-      <c r="CQ1" s="33"/>
-      <c r="CR1" s="33"/>
-      <c r="CS1" s="33"/>
-      <c r="CT1" s="33">
+      <c r="CM1" s="36"/>
+      <c r="CN1" s="36"/>
+      <c r="CO1" s="36"/>
+      <c r="CP1" s="36"/>
+      <c r="CQ1" s="36"/>
+      <c r="CR1" s="36"/>
+      <c r="CS1" s="36"/>
+      <c r="CT1" s="36">
         <f>CL1+Parameters!$B$5</f>
         <v>66</v>
       </c>
-      <c r="CU1" s="33"/>
-      <c r="CV1" s="33"/>
-      <c r="CW1" s="33"/>
-      <c r="CX1" s="33"/>
-      <c r="CY1" s="33"/>
-      <c r="CZ1" s="33"/>
-      <c r="DA1" s="33"/>
-      <c r="DB1" s="33">
+      <c r="CU1" s="36"/>
+      <c r="CV1" s="36"/>
+      <c r="CW1" s="36"/>
+      <c r="CX1" s="36"/>
+      <c r="CY1" s="36"/>
+      <c r="CZ1" s="36"/>
+      <c r="DA1" s="36"/>
+      <c r="DB1" s="36">
         <f>CT1+Parameters!$B$5</f>
         <v>70</v>
       </c>
-      <c r="DC1" s="33"/>
-      <c r="DD1" s="33"/>
-      <c r="DE1" s="33"/>
-      <c r="DF1" s="33"/>
-      <c r="DG1" s="33"/>
-      <c r="DH1" s="33"/>
-      <c r="DI1" s="33"/>
-      <c r="DJ1" s="33">
+      <c r="DC1" s="36"/>
+      <c r="DD1" s="36"/>
+      <c r="DE1" s="36"/>
+      <c r="DF1" s="36"/>
+      <c r="DG1" s="36"/>
+      <c r="DH1" s="36"/>
+      <c r="DI1" s="36"/>
+      <c r="DJ1" s="36">
         <f>DB1+Parameters!$B$5</f>
         <v>74</v>
       </c>
-      <c r="DK1" s="33"/>
-      <c r="DL1" s="33"/>
-      <c r="DM1" s="33"/>
-      <c r="DN1" s="33"/>
-      <c r="DO1" s="33"/>
-      <c r="DP1" s="33"/>
-      <c r="DQ1" s="33"/>
-      <c r="DR1" s="33">
+      <c r="DK1" s="36"/>
+      <c r="DL1" s="36"/>
+      <c r="DM1" s="36"/>
+      <c r="DN1" s="36"/>
+      <c r="DO1" s="36"/>
+      <c r="DP1" s="36"/>
+      <c r="DQ1" s="36"/>
+      <c r="DR1" s="36">
         <f>DJ1+Parameters!$B$5</f>
         <v>78</v>
       </c>
-      <c r="DS1" s="33"/>
-      <c r="DT1" s="33"/>
-      <c r="DU1" s="33"/>
-      <c r="DV1" s="33"/>
-      <c r="DW1" s="33"/>
-      <c r="DX1" s="33"/>
-      <c r="DY1" s="33"/>
+      <c r="DS1" s="36"/>
+      <c r="DT1" s="36"/>
+      <c r="DU1" s="36"/>
+      <c r="DV1" s="36"/>
+      <c r="DW1" s="36"/>
+      <c r="DX1" s="36"/>
+      <c r="DY1" s="36"/>
     </row>
     <row r="2" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="36">
         <f>0.5/4</f>
         <v>0.125</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36">
         <f>0.5/4</f>
         <v>0.125</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33">
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36">
         <f>0.5/4</f>
         <v>0.125</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33">
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36">
         <f>0.5/4</f>
         <v>0.125</v>
       </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33">
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36">
         <f>0.125/4</f>
         <v>3.125E-2</v>
       </c>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33">
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
+      <c r="AL2" s="36"/>
+      <c r="AM2" s="36"/>
+      <c r="AN2" s="36"/>
+      <c r="AO2" s="36"/>
+      <c r="AP2" s="36">
         <f>0.125/4</f>
         <v>3.125E-2</v>
       </c>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="33"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="33">
+      <c r="AQ2" s="36"/>
+      <c r="AR2" s="36"/>
+      <c r="AS2" s="36"/>
+      <c r="AT2" s="36"/>
+      <c r="AU2" s="36"/>
+      <c r="AV2" s="36"/>
+      <c r="AW2" s="36"/>
+      <c r="AX2" s="36">
         <f>0.125/4</f>
         <v>3.125E-2</v>
       </c>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33">
+      <c r="AY2" s="36"/>
+      <c r="AZ2" s="36"/>
+      <c r="BA2" s="36"/>
+      <c r="BB2" s="36"/>
+      <c r="BC2" s="36"/>
+      <c r="BD2" s="36"/>
+      <c r="BE2" s="36"/>
+      <c r="BF2" s="36">
         <f>0.125/4</f>
         <v>3.125E-2</v>
       </c>
-      <c r="BG2" s="33"/>
-      <c r="BH2" s="33"/>
-      <c r="BI2" s="33"/>
-      <c r="BJ2" s="33"/>
-      <c r="BK2" s="33"/>
-      <c r="BL2" s="33"/>
-      <c r="BM2" s="33"/>
-      <c r="BN2" s="33">
+      <c r="BG2" s="36"/>
+      <c r="BH2" s="36"/>
+      <c r="BI2" s="36"/>
+      <c r="BJ2" s="36"/>
+      <c r="BK2" s="36"/>
+      <c r="BL2" s="36"/>
+      <c r="BM2" s="36"/>
+      <c r="BN2" s="36">
         <f>0.125/4*2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="BO2" s="33"/>
-      <c r="BP2" s="33"/>
-      <c r="BQ2" s="33"/>
-      <c r="BR2" s="33"/>
-      <c r="BS2" s="33"/>
-      <c r="BT2" s="33"/>
-      <c r="BU2" s="33"/>
-      <c r="BV2" s="33">
+      <c r="BO2" s="36"/>
+      <c r="BP2" s="36"/>
+      <c r="BQ2" s="36"/>
+      <c r="BR2" s="36"/>
+      <c r="BS2" s="36"/>
+      <c r="BT2" s="36"/>
+      <c r="BU2" s="36"/>
+      <c r="BV2" s="36">
         <f>0.125/4*2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="BW2" s="33"/>
-      <c r="BX2" s="33"/>
-      <c r="BY2" s="33"/>
-      <c r="BZ2" s="33"/>
-      <c r="CA2" s="33"/>
-      <c r="CB2" s="33"/>
-      <c r="CC2" s="33"/>
-      <c r="CD2" s="33">
+      <c r="BW2" s="36"/>
+      <c r="BX2" s="36"/>
+      <c r="BY2" s="36"/>
+      <c r="BZ2" s="36"/>
+      <c r="CA2" s="36"/>
+      <c r="CB2" s="36"/>
+      <c r="CC2" s="36"/>
+      <c r="CD2" s="36">
         <f>0.125/4*2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="CE2" s="33"/>
-      <c r="CF2" s="33"/>
-      <c r="CG2" s="33"/>
-      <c r="CH2" s="33"/>
-      <c r="CI2" s="33"/>
-      <c r="CJ2" s="33"/>
-      <c r="CK2" s="33"/>
-      <c r="CL2" s="33">
+      <c r="CE2" s="36"/>
+      <c r="CF2" s="36"/>
+      <c r="CG2" s="36"/>
+      <c r="CH2" s="36"/>
+      <c r="CI2" s="36"/>
+      <c r="CJ2" s="36"/>
+      <c r="CK2" s="36"/>
+      <c r="CL2" s="36">
         <f>0.125/4*2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="CM2" s="33"/>
-      <c r="CN2" s="33"/>
-      <c r="CO2" s="33"/>
-      <c r="CP2" s="33"/>
-      <c r="CQ2" s="33"/>
-      <c r="CR2" s="33"/>
-      <c r="CS2" s="33"/>
-      <c r="CT2" s="33">
+      <c r="CM2" s="36"/>
+      <c r="CN2" s="36"/>
+      <c r="CO2" s="36"/>
+      <c r="CP2" s="36"/>
+      <c r="CQ2" s="36"/>
+      <c r="CR2" s="36"/>
+      <c r="CS2" s="36"/>
+      <c r="CT2" s="36">
         <f>0.125/4</f>
         <v>3.125E-2</v>
       </c>
-      <c r="CU2" s="33"/>
-      <c r="CV2" s="33"/>
-      <c r="CW2" s="33"/>
-      <c r="CX2" s="33"/>
-      <c r="CY2" s="33"/>
-      <c r="CZ2" s="33"/>
-      <c r="DA2" s="33"/>
-      <c r="DB2" s="33">
+      <c r="CU2" s="36"/>
+      <c r="CV2" s="36"/>
+      <c r="CW2" s="36"/>
+      <c r="CX2" s="36"/>
+      <c r="CY2" s="36"/>
+      <c r="CZ2" s="36"/>
+      <c r="DA2" s="36"/>
+      <c r="DB2" s="36">
         <f>0.125/4</f>
         <v>3.125E-2</v>
       </c>
-      <c r="DC2" s="33"/>
-      <c r="DD2" s="33"/>
-      <c r="DE2" s="33"/>
-      <c r="DF2" s="33"/>
-      <c r="DG2" s="33"/>
-      <c r="DH2" s="33"/>
-      <c r="DI2" s="33"/>
-      <c r="DJ2" s="33">
+      <c r="DC2" s="36"/>
+      <c r="DD2" s="36"/>
+      <c r="DE2" s="36"/>
+      <c r="DF2" s="36"/>
+      <c r="DG2" s="36"/>
+      <c r="DH2" s="36"/>
+      <c r="DI2" s="36"/>
+      <c r="DJ2" s="36">
         <f>0.125/4</f>
         <v>3.125E-2</v>
       </c>
-      <c r="DK2" s="33"/>
-      <c r="DL2" s="33"/>
-      <c r="DM2" s="33"/>
-      <c r="DN2" s="33"/>
-      <c r="DO2" s="33"/>
-      <c r="DP2" s="33"/>
-      <c r="DQ2" s="33"/>
-      <c r="DR2" s="33">
+      <c r="DK2" s="36"/>
+      <c r="DL2" s="36"/>
+      <c r="DM2" s="36"/>
+      <c r="DN2" s="36"/>
+      <c r="DO2" s="36"/>
+      <c r="DP2" s="36"/>
+      <c r="DQ2" s="36"/>
+      <c r="DR2" s="36">
         <f>0.125/4</f>
         <v>3.125E-2</v>
       </c>
-      <c r="DS2" s="33"/>
-      <c r="DT2" s="33"/>
-      <c r="DU2" s="33"/>
-      <c r="DV2" s="33"/>
-      <c r="DW2" s="33"/>
-      <c r="DX2" s="33"/>
-      <c r="DY2" s="33"/>
+      <c r="DS2" s="36"/>
+      <c r="DT2" s="36"/>
+      <c r="DU2" s="36"/>
+      <c r="DV2" s="36"/>
+      <c r="DW2" s="36"/>
+      <c r="DX2" s="36"/>
+      <c r="DY2" s="36"/>
     </row>
     <row r="3" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="37">
         <v>2</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="39">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="37">
         <v>2</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="39">
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="37">
         <v>2</v>
       </c>
-      <c r="S3" s="40"/>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="40"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="39">
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="37">
         <v>2</v>
       </c>
-      <c r="AA3" s="40"/>
-      <c r="AB3" s="40"/>
-      <c r="AC3" s="40"/>
-      <c r="AD3" s="40"/>
-      <c r="AE3" s="40"/>
-      <c r="AF3" s="40"/>
-      <c r="AG3" s="41"/>
-      <c r="AH3" s="39">
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="37">
         <v>6</v>
       </c>
-      <c r="AI3" s="40"/>
-      <c r="AJ3" s="40"/>
-      <c r="AK3" s="40"/>
-      <c r="AL3" s="40"/>
-      <c r="AM3" s="40"/>
-      <c r="AN3" s="40"/>
-      <c r="AO3" s="41"/>
-      <c r="AP3" s="39">
+      <c r="AI3" s="38"/>
+      <c r="AJ3" s="38"/>
+      <c r="AK3" s="38"/>
+      <c r="AL3" s="38"/>
+      <c r="AM3" s="38"/>
+      <c r="AN3" s="38"/>
+      <c r="AO3" s="39"/>
+      <c r="AP3" s="37">
         <v>6</v>
       </c>
-      <c r="AQ3" s="40"/>
-      <c r="AR3" s="40"/>
-      <c r="AS3" s="40"/>
-      <c r="AT3" s="40"/>
-      <c r="AU3" s="40"/>
-      <c r="AV3" s="40"/>
-      <c r="AW3" s="41"/>
-      <c r="AX3" s="39">
+      <c r="AQ3" s="38"/>
+      <c r="AR3" s="38"/>
+      <c r="AS3" s="38"/>
+      <c r="AT3" s="38"/>
+      <c r="AU3" s="38"/>
+      <c r="AV3" s="38"/>
+      <c r="AW3" s="39"/>
+      <c r="AX3" s="37">
         <v>6</v>
       </c>
-      <c r="AY3" s="40"/>
-      <c r="AZ3" s="40"/>
-      <c r="BA3" s="40"/>
-      <c r="BB3" s="40"/>
-      <c r="BC3" s="40"/>
-      <c r="BD3" s="40"/>
-      <c r="BE3" s="41"/>
-      <c r="BF3" s="39">
+      <c r="AY3" s="38"/>
+      <c r="AZ3" s="38"/>
+      <c r="BA3" s="38"/>
+      <c r="BB3" s="38"/>
+      <c r="BC3" s="38"/>
+      <c r="BD3" s="38"/>
+      <c r="BE3" s="39"/>
+      <c r="BF3" s="37">
         <v>6</v>
       </c>
-      <c r="BG3" s="40"/>
-      <c r="BH3" s="40"/>
-      <c r="BI3" s="40"/>
-      <c r="BJ3" s="40"/>
-      <c r="BK3" s="40"/>
-      <c r="BL3" s="40"/>
-      <c r="BM3" s="41"/>
-      <c r="BN3" s="42">
+      <c r="BG3" s="38"/>
+      <c r="BH3" s="38"/>
+      <c r="BI3" s="38"/>
+      <c r="BJ3" s="38"/>
+      <c r="BK3" s="38"/>
+      <c r="BL3" s="38"/>
+      <c r="BM3" s="39"/>
+      <c r="BN3" s="40">
         <v>10</v>
       </c>
-      <c r="BO3" s="37"/>
-      <c r="BP3" s="37"/>
-      <c r="BQ3" s="37"/>
-      <c r="BR3" s="37"/>
-      <c r="BS3" s="37"/>
-      <c r="BT3" s="37"/>
-      <c r="BU3" s="38"/>
-      <c r="BV3" s="36">
+      <c r="BO3" s="41"/>
+      <c r="BP3" s="41"/>
+      <c r="BQ3" s="41"/>
+      <c r="BR3" s="41"/>
+      <c r="BS3" s="41"/>
+      <c r="BT3" s="41"/>
+      <c r="BU3" s="42"/>
+      <c r="BV3" s="43">
         <v>10</v>
       </c>
-      <c r="BW3" s="37"/>
-      <c r="BX3" s="37"/>
-      <c r="BY3" s="37"/>
-      <c r="BZ3" s="37"/>
-      <c r="CA3" s="37"/>
-      <c r="CB3" s="37"/>
-      <c r="CC3" s="38"/>
-      <c r="CD3" s="36">
+      <c r="BW3" s="41"/>
+      <c r="BX3" s="41"/>
+      <c r="BY3" s="41"/>
+      <c r="BZ3" s="41"/>
+      <c r="CA3" s="41"/>
+      <c r="CB3" s="41"/>
+      <c r="CC3" s="42"/>
+      <c r="CD3" s="43">
         <v>10</v>
       </c>
-      <c r="CE3" s="37"/>
-      <c r="CF3" s="37"/>
-      <c r="CG3" s="37"/>
-      <c r="CH3" s="37"/>
-      <c r="CI3" s="37"/>
-      <c r="CJ3" s="37"/>
-      <c r="CK3" s="38"/>
-      <c r="CL3" s="36">
+      <c r="CE3" s="41"/>
+      <c r="CF3" s="41"/>
+      <c r="CG3" s="41"/>
+      <c r="CH3" s="41"/>
+      <c r="CI3" s="41"/>
+      <c r="CJ3" s="41"/>
+      <c r="CK3" s="42"/>
+      <c r="CL3" s="43">
         <v>10</v>
       </c>
-      <c r="CM3" s="37"/>
-      <c r="CN3" s="37"/>
-      <c r="CO3" s="37"/>
-      <c r="CP3" s="37"/>
-      <c r="CQ3" s="37"/>
-      <c r="CR3" s="37"/>
-      <c r="CS3" s="38"/>
-      <c r="CT3" s="36">
+      <c r="CM3" s="41"/>
+      <c r="CN3" s="41"/>
+      <c r="CO3" s="41"/>
+      <c r="CP3" s="41"/>
+      <c r="CQ3" s="41"/>
+      <c r="CR3" s="41"/>
+      <c r="CS3" s="42"/>
+      <c r="CT3" s="43">
         <v>14</v>
       </c>
-      <c r="CU3" s="37"/>
-      <c r="CV3" s="37"/>
-      <c r="CW3" s="37"/>
-      <c r="CX3" s="37"/>
-      <c r="CY3" s="37"/>
-      <c r="CZ3" s="37"/>
-      <c r="DA3" s="38"/>
-      <c r="DB3" s="36">
+      <c r="CU3" s="41"/>
+      <c r="CV3" s="41"/>
+      <c r="CW3" s="41"/>
+      <c r="CX3" s="41"/>
+      <c r="CY3" s="41"/>
+      <c r="CZ3" s="41"/>
+      <c r="DA3" s="42"/>
+      <c r="DB3" s="43">
         <v>14</v>
       </c>
-      <c r="DC3" s="37"/>
-      <c r="DD3" s="37"/>
-      <c r="DE3" s="37"/>
-      <c r="DF3" s="37"/>
-      <c r="DG3" s="37"/>
-      <c r="DH3" s="37"/>
-      <c r="DI3" s="38"/>
-      <c r="DJ3" s="36">
+      <c r="DC3" s="41"/>
+      <c r="DD3" s="41"/>
+      <c r="DE3" s="41"/>
+      <c r="DF3" s="41"/>
+      <c r="DG3" s="41"/>
+      <c r="DH3" s="41"/>
+      <c r="DI3" s="42"/>
+      <c r="DJ3" s="43">
         <v>14</v>
       </c>
-      <c r="DK3" s="37"/>
-      <c r="DL3" s="37"/>
-      <c r="DM3" s="37"/>
-      <c r="DN3" s="37"/>
-      <c r="DO3" s="37"/>
-      <c r="DP3" s="37"/>
-      <c r="DQ3" s="38"/>
-      <c r="DR3" s="36">
+      <c r="DK3" s="41"/>
+      <c r="DL3" s="41"/>
+      <c r="DM3" s="41"/>
+      <c r="DN3" s="41"/>
+      <c r="DO3" s="41"/>
+      <c r="DP3" s="41"/>
+      <c r="DQ3" s="42"/>
+      <c r="DR3" s="43">
         <v>14</v>
       </c>
-      <c r="DS3" s="37"/>
-      <c r="DT3" s="37"/>
-      <c r="DU3" s="37"/>
-      <c r="DV3" s="37"/>
-      <c r="DW3" s="37"/>
-      <c r="DX3" s="37"/>
-      <c r="DY3" s="38"/>
+      <c r="DS3" s="41"/>
+      <c r="DT3" s="41"/>
+      <c r="DU3" s="41"/>
+      <c r="DV3" s="41"/>
+      <c r="DW3" s="41"/>
+      <c r="DX3" s="41"/>
+      <c r="DY3" s="42"/>
     </row>
     <row r="4" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -10842,41 +10834,35 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AH4:AK4"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="AP4:AS4"/>
-    <mergeCell ref="AT4:AW4"/>
-    <mergeCell ref="AX4:BA4"/>
-    <mergeCell ref="BB4:BE4"/>
-    <mergeCell ref="BF4:BI4"/>
-    <mergeCell ref="BJ4:BM4"/>
-    <mergeCell ref="BN4:BQ4"/>
-    <mergeCell ref="BR4:BU4"/>
-    <mergeCell ref="BV4:BY4"/>
-    <mergeCell ref="BZ4:CC4"/>
-    <mergeCell ref="CD4:CG4"/>
-    <mergeCell ref="CH4:CK4"/>
-    <mergeCell ref="CL4:CO4"/>
-    <mergeCell ref="CP4:CS4"/>
-    <mergeCell ref="CT4:CW4"/>
-    <mergeCell ref="CX4:DA4"/>
-    <mergeCell ref="DB4:DE4"/>
-    <mergeCell ref="DF4:DI4"/>
-    <mergeCell ref="DJ4:DM4"/>
+    <mergeCell ref="DB2:DI2"/>
+    <mergeCell ref="DJ2:DQ2"/>
+    <mergeCell ref="DR2:DY2"/>
+    <mergeCell ref="BN2:BU2"/>
+    <mergeCell ref="BV2:CC2"/>
+    <mergeCell ref="CD2:CK2"/>
+    <mergeCell ref="CL2:CS2"/>
+    <mergeCell ref="CT2:DA2"/>
+    <mergeCell ref="Z2:AG2"/>
+    <mergeCell ref="AH2:AO2"/>
+    <mergeCell ref="AP2:AW2"/>
+    <mergeCell ref="AX2:BE2"/>
+    <mergeCell ref="BF2:BM2"/>
+    <mergeCell ref="DR3:DY3"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="AH1:AO1"/>
+    <mergeCell ref="AP1:AW1"/>
+    <mergeCell ref="AX1:BE1"/>
+    <mergeCell ref="BF1:BM1"/>
+    <mergeCell ref="BN1:BU1"/>
+    <mergeCell ref="BV1:CC1"/>
+    <mergeCell ref="CD1:CK1"/>
+    <mergeCell ref="CL1:CS1"/>
+    <mergeCell ref="CT1:DA1"/>
+    <mergeCell ref="DB1:DI1"/>
+    <mergeCell ref="DJ1:DQ1"/>
+    <mergeCell ref="DR1:DY1"/>
+    <mergeCell ref="R2:Y2"/>
     <mergeCell ref="DN4:DQ4"/>
     <mergeCell ref="DR4:DU4"/>
     <mergeCell ref="DV4:DY4"/>
@@ -10893,35 +10879,41 @@
     <mergeCell ref="CT3:DA3"/>
     <mergeCell ref="DB3:DI3"/>
     <mergeCell ref="DJ3:DQ3"/>
-    <mergeCell ref="DR3:DY3"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="AH1:AO1"/>
-    <mergeCell ref="AP1:AW1"/>
-    <mergeCell ref="AX1:BE1"/>
-    <mergeCell ref="BF1:BM1"/>
-    <mergeCell ref="BN1:BU1"/>
-    <mergeCell ref="BV1:CC1"/>
-    <mergeCell ref="CD1:CK1"/>
-    <mergeCell ref="CL1:CS1"/>
-    <mergeCell ref="CT1:DA1"/>
-    <mergeCell ref="DB1:DI1"/>
-    <mergeCell ref="DJ1:DQ1"/>
-    <mergeCell ref="DR1:DY1"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="Z2:AG2"/>
-    <mergeCell ref="AH2:AO2"/>
-    <mergeCell ref="AP2:AW2"/>
-    <mergeCell ref="AX2:BE2"/>
-    <mergeCell ref="BF2:BM2"/>
-    <mergeCell ref="DB2:DI2"/>
-    <mergeCell ref="DJ2:DQ2"/>
-    <mergeCell ref="DR2:DY2"/>
-    <mergeCell ref="BN2:BU2"/>
-    <mergeCell ref="BV2:CC2"/>
-    <mergeCell ref="CD2:CK2"/>
-    <mergeCell ref="CL2:CS2"/>
-    <mergeCell ref="CT2:DA2"/>
+    <mergeCell ref="CT4:CW4"/>
+    <mergeCell ref="CX4:DA4"/>
+    <mergeCell ref="DB4:DE4"/>
+    <mergeCell ref="DF4:DI4"/>
+    <mergeCell ref="DJ4:DM4"/>
+    <mergeCell ref="BZ4:CC4"/>
+    <mergeCell ref="CD4:CG4"/>
+    <mergeCell ref="CH4:CK4"/>
+    <mergeCell ref="CL4:CO4"/>
+    <mergeCell ref="CP4:CS4"/>
+    <mergeCell ref="BF4:BI4"/>
+    <mergeCell ref="BJ4:BM4"/>
+    <mergeCell ref="BN4:BQ4"/>
+    <mergeCell ref="BR4:BU4"/>
+    <mergeCell ref="BV4:BY4"/>
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="AP4:AS4"/>
+    <mergeCell ref="AT4:AW4"/>
+    <mergeCell ref="AX4:BA4"/>
+    <mergeCell ref="BB4:BE4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="J3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>